<commit_message>
Update 2017-2023 comp results.xlsx
</commit_message>
<xml_diff>
--- a/2017-2023 comp results.xlsx
+++ b/2017-2023 comp results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\jomama_lapsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BECBDE-E4DC-4983-933E-DFFABE4B10A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F600BE97-B9AD-4EB1-BC54-BD3885E01908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7E0C2F69-6560-D24A-8FD6-1B7E33CE1C9D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7E0C2F69-6560-D24A-8FD6-1B7E33CE1C9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tmin Tmax" sheetId="6" r:id="rId1"/>
-    <sheet name="2022" sheetId="1" r:id="rId2"/>
-    <sheet name="2019" sheetId="2" r:id="rId3"/>
+    <sheet name="Points Calculator" sheetId="7" r:id="rId2"/>
+    <sheet name="2022" sheetId="1" r:id="rId3"/>
+    <sheet name="2019" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>place</t>
   </si>
@@ -74,13 +75,58 @@
   </si>
   <si>
     <t>Times Scaled for lapsim</t>
+  </si>
+  <si>
+    <t>sweep</t>
+  </si>
+  <si>
+    <t>gear_ratio</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>endurance_battery_capacity</t>
+  </si>
+  <si>
+    <t>endurance time</t>
+  </si>
+  <si>
+    <t>endurance total time</t>
+  </si>
+  <si>
+    <t>autocross time</t>
+  </si>
+  <si>
+    <t>skidpad time</t>
+  </si>
+  <si>
+    <t>acceleration time</t>
+  </si>
+  <si>
+    <t>endurance points</t>
+  </si>
+  <si>
+    <t>autocross points</t>
+  </si>
+  <si>
+    <t>skidpad points</t>
+  </si>
+  <si>
+    <t>acceleration points</t>
+  </si>
+  <si>
+    <t>Total Points</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,8 +135,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -153,23 +214,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{CDF7A488-D468-4B93-9B02-ADD537BAA8D8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3600F42B-D031-0649-BE13-361CE7AF781D}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -497,7 +563,7 @@
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1">
         <v>2023</v>
       </c>
       <c r="C1">
@@ -518,10 +584,10 @@
       <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="7"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -648,7 +714,7 @@
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>2023</v>
       </c>
       <c r="C7">
@@ -813,6 +879,213 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7616863B-A8F4-461E-AD75-7A2338203BF7}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.796875" style="7"/>
+    <col min="2" max="2" width="9.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.8984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.09765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.8984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.09765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.19921875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.796875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="7" t="e">
+        <f>250*((('Tmin Tmax'!$J$11/F2)-1)/(('Tmin Tmax'!$J$11/'Tmin Tmax'!$J$5)-1))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" s="7" t="e">
+        <f>118.5*((('Tmin Tmax'!$J$10/G2)-1)/(('Tmin Tmax'!$J$10/'Tmin Tmax'!$J$4)-1))+6.5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L2" s="7" t="e">
+        <f>71.5*(((('Tmin Tmax'!$J$9/H2)^2)-1)/((('Tmin Tmax'!$J$9/'Tmin Tmax'!$J$3)^2)-1))+3.5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M2" s="7" t="e">
+        <f>95.5*((('Tmin Tmax'!$J$8/I2)-1)/(('Tmin Tmax'!$J$8/'Tmin Tmax'!$J$2)-1))+4.5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N2" s="8" t="e">
+        <f>SUM(J2:M2)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD21AFB-0373-464A-9770-2899E6FA889B}">
   <dimension ref="A1:I14"/>
   <sheetViews>
@@ -1079,7 +1352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C02EC37-504B-FA44-B454-877C97A4147B}">
   <dimension ref="A1:I14"/>
   <sheetViews>

</xml_diff>